<commit_message>
Bugfix: S6 floating point problem fixed. Edit: item data fixed for kg and L.
</commit_message>
<xml_diff>
--- a/solid/Items.xlsx
+++ b/solid/Items.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
   <si>
     <t>water</t>
   </si>
@@ -533,6 +533,10 @@
   </si>
   <si>
     <t>이를 닦는 데 사용된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -942,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -981,10 +985,10 @@
         <v>48</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
         <v>75</v>
@@ -1004,10 +1008,10 @@
         <v>46</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E3" t="s">
         <v>76</v>
@@ -1027,10 +1031,10 @@
         <v>44</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -1050,7 +1054,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1073,7 +1077,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1093,10 +1097,10 @@
         <v>38</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="s">
         <v>57</v>
@@ -1113,10 +1117,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F8" t="s">
         <v>73</v>
@@ -1133,7 +1137,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1153,10 +1157,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F10" t="s">
         <v>68</v>
@@ -1173,10 +1177,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F11" t="s">
         <v>63</v>
@@ -1193,10 +1197,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>71</v>
@@ -1213,10 +1217,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -1233,7 +1237,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1253,10 +1257,10 @@
         <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -1273,10 +1277,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
         <v>69</v>
@@ -1285,7 +1289,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1293,7 +1297,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1305,7 +1309,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1313,10 +1317,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
         <v>72</v>
@@ -1325,7 +1329,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1333,10 +1337,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
         <v>72</v>
@@ -1345,7 +1349,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1353,7 +1357,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -1364,8 +1368,11 @@
       <c r="G20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="K20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1373,10 +1380,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -1385,7 +1392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1393,10 +1400,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="1">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F22" t="s">
         <v>69</v>
@@ -1405,7 +1412,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1413,10 +1420,10 @@
         <v>6</v>
       </c>
       <c r="C23" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
         <v>73</v>
@@ -1425,7 +1432,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1433,10 +1440,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
         <v>74</v>
@@ -1445,7 +1452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1453,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
@@ -1465,7 +1472,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1473,10 +1480,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
         <v>68</v>
@@ -1485,7 +1492,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>

</xml_diff>

<commit_message>
Revert "Bugfix: S6 floating point problem fixed. Edit: item data fixed for kg and L."
This reverts commit 0be579daa8a8111a64d0d39c9f8aba5d469df62a.
</commit_message>
<xml_diff>
--- a/solid/Items.xlsx
+++ b/solid/Items.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>water</t>
   </si>
@@ -533,10 +533,6 @@
   </si>
   <si>
     <t>이를 닦는 데 사용된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -946,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -985,10 +981,10 @@
         <v>48</v>
       </c>
       <c r="C2" s="1">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>75</v>
@@ -1008,10 +1004,10 @@
         <v>46</v>
       </c>
       <c r="C3" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>76</v>
@@ -1031,10 +1027,10 @@
         <v>44</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -1054,7 +1050,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1077,7 +1073,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1097,10 +1093,10 @@
         <v>38</v>
       </c>
       <c r="C7" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>57</v>
@@ -1117,10 +1113,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
         <v>73</v>
@@ -1137,7 +1133,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1157,10 +1153,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>68</v>
@@ -1177,10 +1173,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>63</v>
@@ -1197,10 +1193,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>71</v>
@@ -1217,10 +1213,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -1237,7 +1233,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1257,10 +1253,10 @@
         <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -1277,10 +1273,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
         <v>69</v>
@@ -1289,7 +1285,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1297,7 +1293,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="1">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1309,7 +1305,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1317,10 +1313,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
         <v>72</v>
@@ -1329,7 +1325,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1337,10 +1333,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
         <v>72</v>
@@ -1349,7 +1345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1357,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -1368,11 +1364,8 @@
       <c r="G20" t="s">
         <v>64</v>
       </c>
-      <c r="K20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1380,10 +1373,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -1392,7 +1385,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1400,10 +1393,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="1">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
         <v>69</v>
@@ -1412,7 +1405,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1420,10 +1413,10 @@
         <v>6</v>
       </c>
       <c r="C23" s="1">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1">
         <v>2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>3</v>
       </c>
       <c r="F23" t="s">
         <v>73</v>
@@ -1432,7 +1425,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1440,10 +1433,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D24" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
         <v>74</v>
@@ -1452,7 +1445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1460,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
@@ -1472,7 +1465,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1480,10 +1473,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
         <v>68</v>
@@ -1492,7 +1485,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>

</xml_diff>

<commit_message>
Edit: Items.xlsx description added
</commit_message>
<xml_diff>
--- a/solid/Items.xlsx
+++ b/solid/Items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
   <si>
     <t>korName</t>
   </si>
@@ -54,7 +54,7 @@
     <t>cigs</t>
   </si>
   <si>
-    <t>흡연자의 영원한 친구</t>
+    <t>스트레스를 일시적으로 해소시켜주지만, 건강에는 해로운 아이템입니다.</t>
   </si>
   <si>
     <t>personal_care</t>
@@ -80,7 +80,7 @@
     <t>zipbags</t>
   </si>
   <si>
-    <t>방수를 위해 물건을 보관할 수 있다.</t>
+    <t>음식과 중요한 물건들을 습기로부터 보호할 수 있는 유용한 수납도구입니다.</t>
   </si>
   <si>
     <t>의류</t>
@@ -103,7 +103,7 @@
     <t>paste</t>
   </si>
   <si>
-    <t>이를 닦는 데 사용된다.</t>
+    <t>구강 위생을 유지하여 스트레스를 감소시키는 데 도움을 줍니다.</t>
   </si>
   <si>
     <r>
@@ -123,6 +123,9 @@
     <t>ebrush</t>
   </si>
   <si>
+    <t>효율적인 양치질로 구강 위생을 관리할 수 있지만, 배터리가 필요합니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -140,6 +143,9 @@
     <t>milkbottle</t>
   </si>
   <si>
+    <t>영유아를 위한 필수품이지만, 다른 용도로는 활용도가 낮습니다.</t>
+  </si>
+  <si>
     <t>baby</t>
   </si>
   <si>
@@ -163,6 +169,9 @@
     <t>wallet</t>
   </si>
   <si>
+    <t>현금과 신분증을 보관할 수 있어 비상시에 유용합니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -180,6 +189,9 @@
     <t>lighter</t>
   </si>
   <si>
+    <t>불을 피울 수 있어 음식 조리나 야간 조명으로 활용 가능합니다.</t>
+  </si>
+  <si>
     <t>light</t>
   </si>
   <si>
@@ -200,6 +212,9 @@
     <t>towel</t>
   </si>
   <si>
+    <t>다용도로 활용 가능한 필수품으로, 청결 유지에 도움을 줍니다.</t>
+  </si>
+  <si>
     <t>waterproof</t>
   </si>
   <si>
@@ -220,6 +235,9 @@
     <t>coffee</t>
   </si>
   <si>
+    <t>카페인 섭취로 피로도를 감소시키고 정신을 맑게 해줍니다.</t>
+  </si>
+  <si>
     <t>drink</t>
   </si>
   <si>
@@ -243,6 +261,9 @@
     <t>tuna</t>
   </si>
   <si>
+    <t>단백질이 풍부한 비상식량으로, 오랫동안 보관이 가능합니다.</t>
+  </si>
+  <si>
     <t>food</t>
   </si>
   <si>
@@ -263,6 +284,9 @@
     <t>shoes</t>
   </si>
   <si>
+    <t>발을 보호하고 빠른 이동을 가능하게 하는 필수 아이템입니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -280,6 +304,9 @@
     <t>pants</t>
   </si>
   <si>
+    <t>체온 유지와 신체 보호에 도움을 주는 기본 의류입니다.</t>
+  </si>
+  <si>
     <t>clothing</t>
   </si>
   <si>
@@ -300,6 +327,9 @@
     <t>opener</t>
   </si>
   <si>
+    <t>통조림을 열 수 있게 해주는 필수 도구입니다.</t>
+  </si>
+  <si>
     <t>tool</t>
   </si>
   <si>
@@ -320,6 +350,9 @@
     <t>sweater</t>
   </si>
   <si>
+    <t>추위를 막아주고 체온을 유지시켜주는 따뜻한 의류입니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -337,6 +370,9 @@
     <t>radio</t>
   </si>
   <si>
+    <t>재난 정보와 뉴스를 실시간으로 수신할 수 있는 중요한 통신 도구입니다.</t>
+  </si>
+  <si>
     <t>info</t>
   </si>
   <si>
@@ -360,6 +396,9 @@
     <t>ramen</t>
   </si>
   <si>
+    <t>빠르게 조리 가능한 간편식이지만, 물과 열이 필요합니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -520,6 +559,9 @@
   </si>
   <si>
     <t>water</t>
+  </si>
+  <si>
+    <t>가장 기본적인 수분 공급원입니다.</t>
   </si>
 </sst>
 </file>
@@ -527,7 +569,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +581,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -592,8 +640,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -918,7 +966,7 @@
     <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -964,7 +1012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1010,7 +1058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1024,7 +1072,7 @@
         <v>0.5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>10</v>
@@ -1033,12 +1081,12 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5">
         <v>0.5</v>
@@ -1046,20 +1094,22 @@
       <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5">
         <v>0.5</v>
@@ -1067,7 +1117,9 @@
       <c r="D7" s="5">
         <v>0.5</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1075,12 +1127,12 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5">
         <v>0.1</v>
@@ -1088,20 +1140,22 @@
       <c r="D8" s="5">
         <v>0.1</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5">
         <v>0.5</v>
@@ -1109,20 +1163,22 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5">
         <v>0.5</v>
@@ -1130,20 +1186,22 @@
       <c r="D10" s="5">
         <v>0.5</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
       <c r="A11" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5">
         <v>0.5</v>
@@ -1151,20 +1209,22 @@
       <c r="D11" s="5">
         <v>0.5</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21">
       <c r="A12" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1172,20 +1232,22 @@
       <c r="D12" s="5">
         <v>3</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1193,20 +1255,22 @@
       <c r="D13" s="5">
         <v>2</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5">
         <v>0.5</v>
@@ -1214,20 +1278,22 @@
       <c r="D14" s="5">
         <v>0.5</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F14" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21">
       <c r="A15" s="4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C15" s="5">
         <v>0.5</v>
@@ -1235,20 +1301,22 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="F15" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C16" s="5">
         <v>3</v>
@@ -1256,20 +1324,22 @@
       <c r="D16" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="F16" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21">
       <c r="A17" s="4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C17" s="5">
         <v>0.5</v>
@@ -1277,20 +1347,22 @@
       <c r="D17" s="5">
         <v>1</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="F17" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C18" s="5">
         <v>2</v>
@@ -1300,7 +1372,7 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>15</v>
@@ -1308,10 +1380,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1321,7 +1393,7 @@
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>15</v>
@@ -1329,10 +1401,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C20" s="5">
         <v>0.5</v>
@@ -1342,18 +1414,18 @@
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C21" s="5">
         <v>2</v>
@@ -1363,7 +1435,7 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>15</v>
@@ -1371,10 +1443,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1384,18 +1456,18 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5">
         <v>3</v>
@@ -1405,18 +1477,18 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C24" s="5">
         <v>2</v>
@@ -1426,7 +1498,7 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>15</v>
@@ -1434,10 +1506,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
@@ -1447,18 +1519,18 @@
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1466,12 +1538,14 @@
       <c r="D26" s="5">
         <v>1</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="F26" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
Edit: S8 item description show
</commit_message>
<xml_diff>
--- a/solid/Items.xlsx
+++ b/solid/Items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
   <si>
     <t>korName</t>
   </si>
@@ -416,6 +416,9 @@
     <t>raincoat</t>
   </si>
   <si>
+    <t>비와 습기로부터 몸을 보호하는 방수 의류입니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -433,6 +436,9 @@
     <t>umbrella</t>
   </si>
   <si>
+    <t>비를 피할 수 있지만, 강한 바람에는 취약합니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -450,6 +456,9 @@
     <t>snacks</t>
   </si>
   <si>
+    <t>간단한 포만감을 주는 간식이지만, 영양가는 낮습니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -467,6 +476,9 @@
     <t>jumper</t>
   </si>
   <si>
+    <t>추위와 바람을 막아주는 실용적인 외투입니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -484,6 +496,9 @@
     <t>phone</t>
   </si>
   <si>
+    <t>통신과 정보 검색이 가능하지만, 배터리와 통신망이 필요합니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -501,6 +516,9 @@
     <t>lantern</t>
   </si>
   <si>
+    <t>어둠을 밝혀주는 필수품이지만, 배터리가 필요합니다.</t>
+  </si>
+  <si>
     <r>
       <t/>
     </r>
@@ -518,6 +536,9 @@
     <t>sleepbag</t>
   </si>
   <si>
+    <t>야외에서도 안전하게 휴식을 취할 수 있게 해주는 침구입니다.</t>
+  </si>
+  <si>
     <t>sleep</t>
   </si>
   <si>
@@ -538,6 +559,9 @@
     <t>firstaid</t>
   </si>
   <si>
+    <t>기본적인 부상을 치료할 수 있는 의료용품 세트입니다.</t>
+  </si>
+  <si>
     <t>medical</t>
   </si>
   <si>
@@ -561,7 +585,7 @@
     <t>water</t>
   </si>
   <si>
-    <t>가장 기본적인 수분 공급원입니다.</t>
+    <t>생존에 필수적인 깨끗한 식수입니다.</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1394,9 @@
       <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>37</v>
       </c>
@@ -1380,10 +1406,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1391,7 +1417,9 @@
       <c r="D19" s="5">
         <v>3</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1401,10 +1429,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C20" s="5">
         <v>0.5</v>
@@ -1412,7 +1440,9 @@
       <c r="D20" s="5">
         <v>1</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1422,10 +1452,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C21" s="5">
         <v>2</v>
@@ -1433,7 +1463,9 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>53</v>
       </c>
@@ -1443,10 +1475,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1454,7 +1486,9 @@
       <c r="D22" s="5">
         <v>0.5</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="F22" s="3" t="s">
         <v>64</v>
       </c>
@@ -1464,10 +1498,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C23" s="5">
         <v>3</v>
@@ -1475,7 +1509,9 @@
       <c r="D23" s="5">
         <v>2</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>33</v>
       </c>
@@ -1485,10 +1521,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C24" s="5">
         <v>2</v>
@@ -1496,9 +1532,11 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F24" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>15</v>
@@ -1506,10 +1544,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
@@ -1517,20 +1555,22 @@
       <c r="D25" s="5">
         <v>4</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="F25" s="3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1539,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>41</v>

</xml_diff>